<commit_message>
added final BOM with proven parts values; de-cluttered repository; generated HTML BOM
</commit_message>
<xml_diff>
--- a/rev2final/bom/oibus-mini-CCC.xlsx
+++ b/rev2final/bom/oibus-mini-CCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffael/octanis/clients/ethz/ccc-sensor/rev2final/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffael/octanis/clients/eth/ccc-sensor/rev2final/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F20C7C3F-DB18-234B-957F-21CF75BE79F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE09CD64-FF02-AC4B-913A-9A1634E7677B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="14040" yWindow="1360" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="oibus-mini-CCC" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="226">
   <si>
     <t>Reference</t>
   </si>
@@ -684,12 +684,6 @@
     <t>R14 R15 R16 R3</t>
   </si>
   <si>
-    <t>Batch5</t>
-  </si>
-  <si>
-    <t>Batch210</t>
-  </si>
-  <si>
     <t xml:space="preserve">33uF ±20% 25V </t>
   </si>
   <si>
@@ -697,12 +691,27 @@
   </si>
   <si>
     <t>EEEHBE330UAR</t>
+  </si>
+  <si>
+    <t>ordered</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>RC603JR-071K5L</t>
+  </si>
+  <si>
+    <t>R8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1192,10 +1201,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1550,17 +1561,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="4" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
     <col min="5" max="6" width="30.1640625" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
     <col min="8" max="9" width="30.1640625" customWidth="1"/>
@@ -1568,16 +1581,16 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D1" t="s">
-        <v>219</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1617,19 +1630,17 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
-        <f>B2*5</f>
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="D2">
-        <f>B2*210</f>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -1654,19 +1665,17 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <v>420</v>
+      </c>
+      <c r="D3">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C44" si="0">B3*5</f>
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D44" si="1">B3*210</f>
-        <v>420</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -1685,19 +1694,17 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4">
+      <c r="C4">
+        <v>450</v>
+      </c>
+      <c r="D4">
         <v>2</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -1716,22 +1723,20 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F5" t="s">
         <v>32</v>
@@ -1740,26 +1745,24 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B6">
+      <c r="C6">
+        <v>2100</v>
+      </c>
+      <c r="D6">
         <v>10</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>2100</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
@@ -1778,19 +1781,17 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="B7">
+      <c r="C7">
+        <v>850</v>
+      </c>
+      <c r="D7">
         <v>4</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>840</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
@@ -1809,19 +1810,17 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="B8">
+      <c r="C8">
+        <v>450</v>
+      </c>
+      <c r="D8">
         <v>2</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -1840,19 +1839,17 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="B9">
+      <c r="C9">
+        <v>450</v>
+      </c>
+      <c r="D9">
         <v>2</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E9" t="s">
         <v>46</v>
@@ -1871,19 +1868,17 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="B10">
+      <c r="C10">
+        <v>640</v>
+      </c>
+      <c r="D10">
         <v>3</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>630</v>
       </c>
       <c r="E10" t="s">
         <v>50</v>
@@ -1902,19 +1897,17 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -1933,19 +1926,17 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>58</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>250</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>59</v>
@@ -1964,19 +1955,17 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>63</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>64</v>
@@ -1995,19 +1984,17 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>68</v>
@@ -2026,19 +2013,17 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>72</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>209</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>73</v>
@@ -2057,19 +2042,17 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>77</v>
       </c>
-      <c r="B16">
+      <c r="C16">
+        <v>450</v>
+      </c>
+      <c r="D16">
         <v>2</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E16" t="s">
         <v>78</v>
@@ -2088,19 +2071,14 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>71</v>
@@ -2119,19 +2097,17 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
       <c r="C18" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>88</v>
@@ -2150,19 +2126,17 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>91</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>92</v>
@@ -2181,19 +2155,17 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>95</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>50</v>
@@ -2212,19 +2184,17 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>100</v>
@@ -2243,19 +2213,17 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>104</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>105</v>
@@ -2277,19 +2245,17 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>109</v>
       </c>
-      <c r="B23">
+      <c r="C23">
+        <v>420</v>
+      </c>
+      <c r="D23">
         <v>2</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E23" t="s">
         <v>110</v>
@@ -2311,19 +2277,17 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>114</v>
       </c>
-      <c r="B24">
+      <c r="C24">
+        <v>840</v>
+      </c>
+      <c r="D24">
         <v>4</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
-        <v>840</v>
       </c>
       <c r="E24" t="s">
         <v>115</v>
@@ -2342,19 +2306,17 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>217</v>
       </c>
-      <c r="B25">
+      <c r="C25">
+        <v>850</v>
+      </c>
+      <c r="D25">
         <v>4</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
-        <v>840</v>
       </c>
       <c r="E25" t="s">
         <v>119</v>
@@ -2373,22 +2335,20 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>122</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>223</v>
       </c>
       <c r="F26" t="s">
         <v>116</v>
@@ -2396,27 +2356,22 @@
       <c r="G26" t="s">
         <v>17</v>
       </c>
-      <c r="H26" t="s">
-        <v>124</v>
-      </c>
       <c r="I26" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>126</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>250</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>127</v>
@@ -2435,19 +2390,17 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>130</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
       <c r="C28">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>131</v>
@@ -2466,19 +2419,17 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>134</v>
       </c>
-      <c r="B29">
+      <c r="C29">
+        <v>650</v>
+      </c>
+      <c r="D29">
         <v>3</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="1"/>
-        <v>630</v>
       </c>
       <c r="E29" t="s">
         <v>135</v>
@@ -2497,19 +2448,17 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>138</v>
       </c>
-      <c r="B30">
+      <c r="C30">
+        <v>450</v>
+      </c>
+      <c r="D30">
         <v>2</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E30" t="s">
         <v>139</v>
@@ -2528,19 +2477,17 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>142</v>
       </c>
-      <c r="B31">
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
         <v>2</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="1"/>
-        <v>420</v>
       </c>
       <c r="E31" t="s">
         <v>143</v>
@@ -2559,19 +2506,17 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>146</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
       <c r="C32">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
         <v>147</v>
@@ -2590,19 +2535,17 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>151</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
       <c r="C33">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>202</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
         <v>147</v>
@@ -2621,19 +2564,17 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>155</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
       <c r="C34">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
         <v>156</v>
@@ -2652,19 +2593,17 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
       <c r="C35" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>162</v>
@@ -2680,19 +2619,17 @@
       </c>
     </row>
     <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
       <c r="C36" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>166</v>
@@ -2723,19 +2660,17 @@
       </c>
     </row>
     <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
       <c r="C37" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>175</v>
@@ -2766,19 +2701,17 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>181</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
       <c r="C38">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
         <v>182</v>
@@ -2797,19 +2730,17 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>186</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
       <c r="C39">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
         <v>187</v>
@@ -2825,19 +2756,17 @@
       </c>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="C40" s="4">
+        <v>202</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>192</v>
@@ -2868,19 +2797,17 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>197</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="C41" s="3">
+        <v>142</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
         <v>198</v>
@@ -2899,19 +2826,17 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>203</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
       <c r="C42">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
         <v>204</v>
@@ -2930,19 +2855,17 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>207</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
       <c r="C43">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
         <v>208</v>
@@ -2961,19 +2884,17 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>212</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
       <c r="C44">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
         <v>213</v>
@@ -2991,10 +2912,36 @@
         <v>216</v>
       </c>
     </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>225</v>
+      </c>
+      <c r="C45">
+        <v>210</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" t="s">
+        <v>116</v>
+      </c>
+      <c r="H45" t="s">
+        <v>124</v>
+      </c>
+      <c r="I45" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" display="https://lcsc.com/product-detail/Others_PANASONIC-EEEHBE330UAR_C336470.html"/>
-    <hyperlink ref="I5" r:id="rId2" display="https://lcsc.com/product-detail/Others_PANASONIC-EEEHBE330UAR_C336470.html"/>
+    <hyperlink ref="H5" r:id="rId1" display="https://lcsc.com/product-detail/Others_PANASONIC-EEEHBE330UAR_C336470.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I5" r:id="rId2" display="https://lcsc.com/product-detail/Others_PANASONIC-EEEHBE330UAR_C336470.html" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>